<commit_message>
edited R markdown file, created smeg growth curve table
</commit_message>
<xml_diff>
--- a/data/Processed_data/combined_percentinfected.xlsx
+++ b/data/Processed_data/combined_percentinfected.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ousstudent/Documents/Isma_Michael_summer2023/data/Processed_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A445DE61-4225-3E40-941D-53B75686E97C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A594C28-29FA-7449-A29D-B88BF28F0488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15320" xr2:uid="{30182D6F-E94D-244E-AB8F-07510FEAF6C9}"/>
+    <workbookView xWindow="9280" yWindow="9320" windowWidth="27640" windowHeight="15320" xr2:uid="{30182D6F-E94D-244E-AB8F-07510FEAF6C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" iterateDelta="1E-4"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -458,7 +458,7 @@
   <dimension ref="A1:Q31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D1" sqref="D1:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>